<commit_message>
Done Some UI Changes
</commit_message>
<xml_diff>
--- a/backend/vendors/Demo/demo.XLSX
+++ b/backend/vendors/Demo/demo.XLSX
@@ -134,20 +134,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -277,96 +281,96 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>101</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="3" t="n">
         <v>55.99</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="3" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
         <v>102</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>65.99</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="3" t="n">
         <v>103</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>75.99</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="3" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="3" t="n">
         <v>104</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>85.99</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
+      <c r="A6" s="3" t="n">
         <v>105</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>95.99</v>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>30</v>
+      <c r="D6" s="3" t="n">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>